<commit_message>
Committing db structure changes
</commit_message>
<xml_diff>
--- a/db-structure.xlsx
+++ b/db-structure.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
-    <sheet name="teams" sheetId="2" r:id="rId2"/>
-    <sheet name="match-titles" sheetId="3" r:id="rId3"/>
-    <sheet name="matches" sheetId="4" r:id="rId4"/>
-    <sheet name="match-templates" sheetId="7" r:id="rId5"/>
-    <sheet name="scheduled_matches" sheetId="5" r:id="rId6"/>
-    <sheet name="reports" sheetId="6" r:id="rId7"/>
+    <sheet name="courts" sheetId="8" r:id="rId2"/>
+    <sheet name="teams" sheetId="2" r:id="rId3"/>
+    <sheet name="match-titles" sheetId="3" r:id="rId4"/>
+    <sheet name="matches" sheetId="4" r:id="rId5"/>
+    <sheet name="match-templates" sheetId="7" r:id="rId6"/>
+    <sheet name="scheduled_matches" sheetId="5" r:id="rId7"/>
+    <sheet name="reports" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>user_name</t>
   </si>
@@ -122,6 +123,9 @@
   </si>
   <si>
     <t>must be unique</t>
+  </si>
+  <si>
+    <t>court_name</t>
   </si>
 </sst>
 </file>
@@ -576,6 +580,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
@@ -626,7 +684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -669,278 +727,6 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1220,6 +1006,278 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:M14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1389,11 +1447,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>

</xml_diff>